<commit_message>
Big changes: 'finished' draft of the Monty class, and started applying it to the IFRC GO Emergency Appeal database. Changes in the taxonomy have also been made.
</commit_message>
<xml_diff>
--- a/Taxonomies/MostlyImpactData/GIDD-HIP.xlsx
+++ b/Taxonomies/MostlyImpactData/GIDD-HIP.xlsx
@@ -312,7 +312,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -337,10 +337,17 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="11"/>
+      <sz val="8"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
@@ -393,12 +400,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -410,7 +421,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -434,12 +445,23 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="44.97"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -465,7 +487,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -487,7 +509,7 @@
       <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -504,7 +526,7 @@
       <c r="D3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -517,7 +539,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -539,11 +561,11 @@
       <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -553,20 +575,21 @@
       <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="D5" s="5"/>
       <c r="E5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -588,7 +611,7 @@
       <c r="G6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -605,15 +628,16 @@
       <c r="D7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
@@ -628,15 +652,16 @@
       <c r="D8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="E8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="4" t="s">
         <v>38</v>
       </c>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
@@ -651,15 +676,16 @@
       <c r="D9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="E9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="4" t="s">
         <v>43</v>
       </c>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
@@ -674,15 +700,16 @@
       <c r="D10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="E10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="4" t="s">
         <v>47</v>
       </c>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
@@ -694,15 +721,17 @@
       <c r="C11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="D11" s="5"/>
+      <c r="E11" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="2" t="s">
         <v>51</v>
       </c>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
@@ -717,15 +746,16 @@
       <c r="D12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="3" t="s">
+      <c r="E12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
@@ -740,15 +770,16 @@
       <c r="D13" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="E13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="4" t="s">
         <v>58</v>
       </c>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
@@ -763,15 +794,16 @@
       <c r="D14" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F14" s="3" t="s">
+      <c r="E14" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="4" t="s">
         <v>62</v>
       </c>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
@@ -786,15 +818,16 @@
       <c r="D15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="3" t="s">
+      <c r="E15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="H15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
@@ -809,15 +842,16 @@
       <c r="D16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="3" t="s">
+      <c r="E16" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
@@ -832,15 +866,16 @@
       <c r="D17" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="3" t="s">
+      <c r="E17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="H17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
@@ -855,15 +890,16 @@
       <c r="D18" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F18" s="3" t="s">
+      <c r="E18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="H18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
@@ -878,15 +914,16 @@
       <c r="D19" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F19" s="3" t="s">
+      <c r="E19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="4" t="s">
         <v>73</v>
       </c>
+      <c r="H19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
@@ -901,15 +938,16 @@
       <c r="D20" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="3" t="s">
+      <c r="E20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="4" t="s">
         <v>77</v>
       </c>
+      <c r="H20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
@@ -924,15 +962,16 @@
       <c r="D21" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F21" s="3" t="s">
+      <c r="E21" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="4" t="s">
         <v>79</v>
       </c>
+      <c r="H21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
@@ -947,12 +986,14 @@
       <c r="D22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
@@ -967,15 +1008,16 @@
       <c r="D23" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="4" t="s">
         <v>85</v>
       </c>
+      <c r="H23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
@@ -990,157 +1032,158 @@
       <c r="D24" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" s="3" t="s">
+      <c r="E24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="4" t="s">
         <v>87</v>
       </c>
+      <c r="H24" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>